<commit_message>
major update of grid scan analysis
</commit_message>
<xml_diff>
--- a/_hydro-radar-grid.xlsx
+++ b/_hydro-radar-grid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giord\Desktop\hrc-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF8EEEA-778E-47D6-B17C-92ECBC842B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E15C95C-EC13-487A-B7A0-D3ED521DF1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C60B9B42-610B-418E-B17A-28126607FE42}"/>
   </bookViews>
@@ -462,6 +462,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -469,15 +478,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2088,7 +2088,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,46 +2958,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C1" s="55">
+      <c r="C1" s="52">
         <f>grid!$A$15</f>
         <v>21.3</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="55">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="52">
         <f>grid!$A$16</f>
         <v>24</v>
       </c>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="55">
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="52">
         <f>grid!$A$17</f>
         <v>27</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="55">
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="52">
         <f>grid!$A$18</f>
         <v>31</v>
       </c>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="55">
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="52">
         <f>grid!$A$19</f>
         <v>35</v>
       </c>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="57"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="54"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C2" s="1">
@@ -3102,7 +3102,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="A3" s="55">
         <f t="shared" ref="A3" si="0">$C$1</f>
         <v>21.3</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="AA3" s="12"/>
     </row>
     <row r="4" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="35">
         <f>$B$3</f>
         <v>1.7230854575774166</v>
@@ -3139,7 +3139,7 @@
       <c r="AA4" s="37"/>
     </row>
     <row r="5" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="35">
         <f t="shared" ref="B5:B7" si="1">$B$3</f>
         <v>1.7230854575774166</v>
@@ -3156,7 +3156,7 @@
       <c r="AA5" s="37"/>
     </row>
     <row r="6" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="35">
         <f t="shared" si="1"/>
         <v>1.7230854575774166</v>
@@ -3173,7 +3173,7 @@
       <c r="AA6" s="37"/>
     </row>
     <row r="7" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="36">
         <f t="shared" si="1"/>
         <v>1.7230854575774166</v>
@@ -3190,7 +3190,7 @@
       <c r="AA7" s="39"/>
     </row>
     <row r="8" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52">
+      <c r="A8" s="55">
         <f t="shared" ref="A8" si="2">$H$1</f>
         <v>24</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="AA8" s="12"/>
     </row>
     <row r="9" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="35">
         <f>B8</f>
         <v>1.5040033964861734</v>
@@ -3227,7 +3227,7 @@
       <c r="AA9" s="37"/>
     </row>
     <row r="10" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="35">
         <f>B8</f>
         <v>1.5040033964861734</v>
@@ -3244,7 +3244,7 @@
       <c r="AA10" s="37"/>
     </row>
     <row r="11" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="35">
         <f>B8</f>
         <v>1.5040033964861734</v>
@@ -3261,7 +3261,7 @@
       <c r="AA11" s="37"/>
     </row>
     <row r="12" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="36">
         <f>B8</f>
         <v>1.5040033964861734</v>
@@ -3278,7 +3278,7 @@
       <c r="AA12" s="39"/>
     </row>
     <row r="13" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52">
+      <c r="A13" s="55">
         <f t="shared" ref="A13" si="3">$M$1</f>
         <v>27</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="AA13" s="12"/>
     </row>
     <row r="14" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="35">
         <f>B13</f>
         <v>1.3089057348643709</v>
@@ -3315,7 +3315,7 @@
       <c r="AA14" s="37"/>
     </row>
     <row r="15" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="35">
         <f>B13</f>
         <v>1.3089057348643709</v>
@@ -3332,7 +3332,7 @@
       <c r="AA15" s="37"/>
     </row>
     <row r="16" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="35">
         <f>B13</f>
         <v>1.3089057348643709</v>
@@ -3349,7 +3349,7 @@
       <c r="AA16" s="37"/>
     </row>
     <row r="17" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="36">
         <f>B13</f>
         <v>1.3089057348643709</v>
@@ -3366,7 +3366,7 @@
       <c r="AA17" s="39"/>
     </row>
     <row r="18" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52">
+      <c r="A18" s="55">
         <f t="shared" ref="A18" si="4">$R$1</f>
         <v>31</v>
       </c>
@@ -3386,7 +3386,7 @@
       <c r="AA18" s="12"/>
     </row>
     <row r="19" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="35">
         <f>$B$18</f>
         <v>1.1031844242963265</v>
@@ -3403,7 +3403,7 @@
       <c r="AA19" s="37"/>
     </row>
     <row r="20" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="35">
         <f t="shared" ref="B20:B22" si="5">$B$18</f>
         <v>1.1031844242963265</v>
@@ -3420,7 +3420,7 @@
       <c r="AA20" s="37"/>
     </row>
     <row r="21" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="35">
         <f t="shared" si="5"/>
         <v>1.1031844242963265</v>
@@ -3437,7 +3437,7 @@
       <c r="AA21" s="37"/>
     </row>
     <row r="22" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="36">
         <f t="shared" si="5"/>
         <v>1.1031844242963265</v>
@@ -3454,7 +3454,7 @@
       <c r="AA22" s="39"/>
     </row>
     <row r="23" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52">
+      <c r="A23" s="55">
         <f t="shared" ref="A23" si="6">$W$1</f>
         <v>35</v>
       </c>
@@ -3474,7 +3474,7 @@
       <c r="AA23" s="12"/>
     </row>
     <row r="24" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="35">
         <f>$B$23</f>
         <v>0.94014732688799052</v>
@@ -3491,7 +3491,7 @@
       <c r="AA24" s="37"/>
     </row>
     <row r="25" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="35">
         <f t="shared" ref="B25:B27" si="7">$B$23</f>
         <v>0.94014732688799052</v>
@@ -3508,7 +3508,7 @@
       <c r="AA25" s="37"/>
     </row>
     <row r="26" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="35">
         <f t="shared" si="7"/>
         <v>0.94014732688799052</v>
@@ -3525,7 +3525,7 @@
       <c r="AA26" s="37"/>
     </row>
     <row r="27" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="36">
         <f t="shared" si="7"/>
         <v>0.94014732688799052</v>
@@ -3543,16 +3543,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A27"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="R1:V1"/>
     <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>